<commit_message>
Organizing my books. Adding notes from Reinforcement Learning Chapter1. Updating Interests.xlsx and Updates.xlsx
</commit_message>
<xml_diff>
--- a/interests/Interests.xlsx
+++ b/interests/Interests.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Google Drive\Master's\Interests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.rucker\My Projects\PTL\mr2an\interests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="733" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="733" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Individuals" sheetId="4" r:id="rId1"/>
@@ -17,8 +17,8 @@
     <sheet name="Organizations" sheetId="6" r:id="rId3"/>
     <sheet name="Journals" sheetId="5" r:id="rId4"/>
     <sheet name="Research" sheetId="2" r:id="rId5"/>
-    <sheet name="Programs" sheetId="3" r:id="rId6"/>
-    <sheet name="Resources" sheetId="7" r:id="rId7"/>
+    <sheet name="Resources" sheetId="7" r:id="rId6"/>
+    <sheet name="Questions" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>Id</t>
   </si>
@@ -189,13 +189,46 @@
   </si>
   <si>
     <t>Epidemic Intelligence Service</t>
+  </si>
+  <si>
+    <t>Mathematical Sociology</t>
+  </si>
+  <si>
+    <t>Computational Sociology</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Are there fundamental formulas that govern social interactions?</t>
+  </si>
+  <si>
+    <t>Did consciousness evolve to priorotize information processing?</t>
+  </si>
+  <si>
+    <t>Can we create mathematical models of social systems?</t>
+  </si>
+  <si>
+    <t>Journal of Mathematical Sociology</t>
+  </si>
+  <si>
+    <t>Social Networks</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>Can we accurately model the impact of an AI application on social networks?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +243,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF252525"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -233,9 +272,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -786,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,35 +940,71 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -937,19 +1013,21 @@
     <hyperlink ref="B4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -965,36 +1043,39 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,4 +1129,55 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="75.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="Did consciousness evolve to priorotize information processing"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating interests adding articles
</commit_message>
<xml_diff>
--- a/interests/Interests.xlsx
+++ b/interests/Interests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="733" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="733" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Individuals" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
   <si>
     <t>Id</t>
   </si>
@@ -378,6 +378,33 @@
   <si>
     <t>Gonçalves, Bruno and Perra, Nicola (eds.)</t>
   </si>
+  <si>
+    <t>B Corporations</t>
+  </si>
+  <si>
+    <t>Comercial business seeking a triple bottom line</t>
+  </si>
+  <si>
+    <t>Ashoka</t>
+  </si>
+  <si>
+    <t>The leader in social entrepreneurship</t>
+  </si>
+  <si>
+    <t>One of the world's most succesfull development NGO's</t>
+  </si>
+  <si>
+    <t>Lots of interesting articles on people addressing social problems</t>
+  </si>
+  <si>
+    <t>Created by Eric Schmidt, the founder of Google</t>
+  </si>
+  <si>
+    <t>Concrete Mathematics</t>
+  </si>
+  <si>
+    <t>Portmanteau of Continuous and Discrete. Written by Knuth.</t>
+  </si>
 </sst>
 </file>
 
@@ -400,15 +427,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF252525"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF252525"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -438,7 +466,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -970,10 +998,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,6 +1036,9 @@
       <c r="B3" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1016,6 +1047,9 @@
       <c r="B4" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1032,6 +1066,9 @@
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1121,6 +1158,28 @@
       </c>
       <c r="C15" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1138,6 +1197,8 @@
     <hyperlink ref="B14" r:id="rId11"/>
     <hyperlink ref="B10" r:id="rId12"/>
     <hyperlink ref="B15" r:id="rId13"/>
+    <hyperlink ref="B16" r:id="rId14"/>
+    <hyperlink ref="B17" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1328,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,6 +1490,17 @@
       </c>
       <c r="D7" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1447,7 +1519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding update, interests and article
</commit_message>
<xml_diff>
--- a/interests/Interests.xlsx
+++ b/interests/Interests.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="733" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="733" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Individuals" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="111">
   <si>
     <t>Id</t>
   </si>
@@ -404,6 +404,12 @@
   </si>
   <si>
     <t>Portmanteau of Continuous and Discrete. Written by Knuth.</t>
+  </si>
+  <si>
+    <t>ideas42</t>
+  </si>
+  <si>
+    <t>Regulation Room</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,6 +1186,22 @@
       </c>
       <c r="C17" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1199,6 +1221,8 @@
     <hyperlink ref="B15" r:id="rId13"/>
     <hyperlink ref="B16" r:id="rId14"/>
     <hyperlink ref="B17" r:id="rId15"/>
+    <hyperlink ref="B18" r:id="rId16"/>
+    <hyperlink ref="B19" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1519,7 +1543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>

</xml_diff>